<commit_message>
add doc link in sample file
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/sample.xlsx
+++ b/src/main/webapp/WEB-INF/books/sample.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27106"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/zssessentials/src/main/webapp/WEB-INF/books/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="17460" windowHeight="9465" tabRatio="781" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="781" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +30,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">AutoFilter!$C$4:$E$11</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="67">
   <si>
     <t>ABC</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -283,48 +296,44 @@
     <t>zkoss http</t>
   </si>
   <si>
-    <t>Mail dennis</t>
-  </si>
-  <si>
-    <t>AAAA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BBBBB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ccc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>toggle merge center here (long long long long text)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>1/13/2013</t>
+  </si>
+  <si>
+    <t>link to AN1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>link to Image!A1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mail Hawk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="177" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -333,7 +342,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -342,7 +351,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF00B050"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -351,7 +360,7 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -359,7 +368,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -367,7 +376,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -381,12 +390,20 @@
       <charset val="136"/>
     </font>
     <font>
-      <sz val="24"/>
+      <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="18"/>
+      <color theme="10"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
     </font>
   </fonts>
   <fills count="5">
@@ -425,37 +442,37 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
         <color rgb="FF00B050"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
         <color rgb="FF00B050"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color rgb="FF00B050"/>
@@ -465,10 +482,10 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color rgb="FF00B050"/>
@@ -477,7 +494,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
         <color rgb="FF00B050"/>
@@ -493,7 +510,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color rgb="FF00B050"/>
@@ -505,11 +522,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -517,22 +534,22 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -540,7 +557,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -550,7 +567,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -592,7 +609,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -626,19 +643,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -653,6 +664,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -660,17 +677,34 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -733,34 +767,500 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300</c:v>
+                  <c:v>300.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400</c:v>
+                  <c:v>400.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600</c:v>
+                  <c:v>600.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700</c:v>
+                  <c:v>700.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800</c:v>
+                  <c:v>800.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Chart Inside'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>K2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Chart Inside'!$B$3:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>F</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>J</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart Inside'!$D$3:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>102.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>276.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>432.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>572.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>432.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>210.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Chart Inside'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>K3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Chart Inside'!$B$3:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>F</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>J</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart Inside'!$E$3:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>875.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>554.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>283.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>843.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>324.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>476.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>123.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>351.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>672.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>772.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Chart Inside'!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SUM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Chart Inside'!$B$3:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>F</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>J</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart Inside'!$F$3:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>798.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>606.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1308.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>926.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1352.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1255.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1723.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2004.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1982.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-2111153392"/>
+        <c:axId val="-2111150304"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2111153392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2111150304"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2111150304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2111153392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Chart Inside'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>K1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Chart Inside'!$B$3:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>F</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>J</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart Inside'!$C$3:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -780,9 +1280,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Chart Inside'!$B$3:$B$12</c:f>
@@ -828,34 +1326,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>33</c:v>
+                  <c:v>33.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44</c:v>
+                  <c:v>44.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>65</c:v>
+                  <c:v>65.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>102</c:v>
+                  <c:v>102.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>276</c:v>
+                  <c:v>276.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>432</c:v>
+                  <c:v>432.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>572</c:v>
+                  <c:v>572.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>432</c:v>
+                  <c:v>432.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>210</c:v>
+                  <c:v>210.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -875,9 +1373,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Chart Inside'!$B$3:$B$12</c:f>
@@ -923,34 +1419,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>875</c:v>
+                  <c:v>875.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>554</c:v>
+                  <c:v>554.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>283</c:v>
+                  <c:v>283.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>843</c:v>
+                  <c:v>843.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>324</c:v>
+                  <c:v>324.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>476</c:v>
+                  <c:v>476.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>123</c:v>
+                  <c:v>123.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>351</c:v>
+                  <c:v>351.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>672</c:v>
+                  <c:v>672.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>772</c:v>
+                  <c:v>772.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -970,9 +1466,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Chart Inside'!$B$3:$B$12</c:f>
@@ -1018,498 +1512,97 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1008</c:v>
+                  <c:v>1008.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>798</c:v>
+                  <c:v>798.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>606</c:v>
+                  <c:v>606.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1308</c:v>
+                  <c:v>1308.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>926</c:v>
+                  <c:v>926.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1352</c:v>
+                  <c:v>1352.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1255</c:v>
+                  <c:v>1255.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1723</c:v>
+                  <c:v>1723.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2004</c:v>
+                  <c:v>2004.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1982</c:v>
+                  <c:v>1982.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="91440256"/>
-        <c:axId val="91442176"/>
-      </c:lineChart>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2111062912"/>
+        <c:axId val="-2111059824"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="91440256"/>
+        <c:axId val="-2111062912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:axPos val="b"/>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91442176"/>
+        <c:crossAx val="-2111059824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91442176"/>
+        <c:axId val="-2111059824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:axPos val="l"/>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91440256"/>
+        <c:crossAx val="-2111062912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Chart Inside'!$C$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>K1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Chart Inside'!$B$3:$B$12</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>A</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>B</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>C</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>D</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>E</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>F</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>G</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>H</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>I</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>J</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Chart Inside'!$C$3:$C$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>600</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>700</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>800</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Chart Inside'!$D$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>K2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Chart Inside'!$B$3:$B$12</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>A</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>B</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>C</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>D</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>E</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>F</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>G</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>H</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>I</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>J</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Chart Inside'!$D$3:$D$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>102</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>276</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>432</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>572</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>432</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>210</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Chart Inside'!$E$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>K3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Chart Inside'!$B$3:$B$12</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>A</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>B</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>C</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>D</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>E</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>F</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>G</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>H</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>I</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>J</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Chart Inside'!$E$3:$E$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>875</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>554</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>283</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>843</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>324</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>476</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>123</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>351</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>672</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>772</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Chart Inside'!$F$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SUM</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Chart Inside'!$B$3:$B$12</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>A</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>B</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>C</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>D</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>E</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>F</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>G</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>H</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>I</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>J</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Chart Inside'!$F$3:$F$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1008</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>798</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>606</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1308</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>926</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1352</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1255</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1723</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1982</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="78215424"/>
-        <c:axId val="78217216"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="78215424"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78217216"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="78217216"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78215424"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1666,12 +1759,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1698,14 +1791,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1732,6 +1826,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1907,33 +2002,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.19921875" customWidth="1"/>
+    <col min="2" max="2" width="14.19921875" customWidth="1"/>
+    <col min="3" max="3" width="12.59765625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.59765625" customWidth="1"/>
+    <col min="6" max="6" width="14.3984375" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" style="8" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.796875" style="8" customWidth="1"/>
+    <col min="9" max="9" width="16.19921875" customWidth="1"/>
+    <col min="10" max="10" width="13.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1941,7 +2036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B4" s="5">
         <v>123</v>
       </c>
@@ -1956,7 +2051,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B5" s="3">
         <v>41375</v>
       </c>
@@ -1964,7 +2059,7 @@
         <v>41375</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="7" customFormat="1">
+    <row r="9" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="G9" s="7" t="s">
         <v>2</v>
       </c>
@@ -1973,22 +2068,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H10" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H13" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="70.5" customHeight="1">
+    <row r="16" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="45">
+    <row r="18" spans="2:4" ht="42" x14ac:dyDescent="0.15">
       <c r="B18" s="17" t="s">
         <v>15</v>
       </c>
@@ -2004,16 +2099,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="2:2">
+    <row r="1" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B1" t="s">
         <v>60</v>
       </c>
@@ -2027,16 +2120,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>3</v>
       </c>
@@ -2065,7 +2158,7 @@
         <v>41275</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B4">
         <v>2</v>
       </c>
@@ -2086,7 +2179,7 @@
         <v>41306</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B5">
         <v>3</v>
       </c>
@@ -2113,20 +2206,20 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.796875" customWidth="1"/>
+    <col min="9" max="9" width="9.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B3" s="21" t="s">
         <v>54</v>
       </c>
@@ -2140,7 +2233,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:11">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B4" s="21" t="s">
         <v>57</v>
       </c>
@@ -2148,7 +2241,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="2:11">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>53</v>
       </c>
@@ -2168,7 +2261,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="2:11">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>55</v>
       </c>
@@ -2182,7 +2275,7 @@
         <v>41305</v>
       </c>
     </row>
-    <row r="8" spans="2:11">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
         <v>58</v>
       </c>
@@ -2224,26 +2317,26 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.796875" customWidth="1"/>
+    <col min="9" max="9" width="9.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B3" s="21"/>
     </row>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B4" s="21"/>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>59</v>
       </c>
@@ -2251,11 +2344,11 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.15">
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C8" s="22"/>
     </row>
   </sheetData>
@@ -2271,38 +2364,41 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="43.28515625" customWidth="1"/>
+    <col min="2" max="2" width="43.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="15.75">
-      <c r="B2" s="23" t="s">
+    <row r="1" spans="2:2" ht="25" x14ac:dyDescent="0.15">
+      <c r="B1" s="27"/>
+    </row>
+    <row r="2" spans="2:2" ht="25" x14ac:dyDescent="0.15">
+      <c r="B2" s="28" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.75">
-      <c r="B3" s="23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3">
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="31.5">
-      <c r="B8" s="24" t="s">
+    <row r="3" spans="2:2" ht="25" x14ac:dyDescent="0.15">
+      <c r="B3" s="28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="25" x14ac:dyDescent="0.15">
+      <c r="B4" s="27"/>
+    </row>
+    <row r="5" spans="2:2" ht="25" x14ac:dyDescent="0.15">
+      <c r="B5" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="24" t="s">
+    </row>
+    <row r="6" spans="2:2" ht="25" x14ac:dyDescent="0.15">
+      <c r="B6" s="28" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2311,6 +2407,8 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B5" location="HyperLink!AN1" display="link to AN1"/>
+    <hyperlink ref="B6" location="Image!A1" display="link to Image!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
@@ -2318,31 +2416,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.19921875" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:5">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C5" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="3:5">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.15">
       <c r="D6" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="3:5">
+    <row r="7" spans="3:5" x14ac:dyDescent="0.15">
       <c r="E7" s="10" t="s">
         <v>7</v>
       </c>
@@ -2356,21 +2454,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="2" spans="3:3">
+    <row r="2" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="3:3">
+    <row r="4" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C4" t="s">
         <v>9</v>
       </c>
@@ -2382,63 +2480,63 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.59765625" customWidth="1"/>
+    <col min="5" max="5" width="11.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:9">
-      <c r="D4" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="26"/>
+    <row r="4" spans="4:9" x14ac:dyDescent="0.15">
+      <c r="D4" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="24"/>
       <c r="G4" s="11" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="15"/>
       <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="4:9">
-      <c r="D5" s="27"/>
-      <c r="E5" s="28"/>
+    <row r="5" spans="4:9" x14ac:dyDescent="0.15">
+      <c r="D5" s="25"/>
+      <c r="E5" s="26"/>
       <c r="G5" s="13"/>
       <c r="H5" s="16"/>
       <c r="I5" s="14"/>
     </row>
-    <row r="7" spans="4:9">
-      <c r="D7" s="25" t="s">
+    <row r="7" spans="4:9" x14ac:dyDescent="0.15">
+      <c r="D7" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="26"/>
+      <c r="E7" s="24"/>
       <c r="G7" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="15"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="4:9">
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.15">
+      <c r="D8" s="25"/>
+      <c r="E8" s="26"/>
       <c r="G8" s="13"/>
       <c r="H8" s="16"/>
       <c r="I8" s="14"/>
     </row>
-    <row r="10" spans="4:9">
+    <row r="10" spans="4:9" x14ac:dyDescent="0.15">
       <c r="D10" s="11" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="12"/>
     </row>
-    <row r="11" spans="4:9">
+    <row r="11" spans="4:9" x14ac:dyDescent="0.15">
       <c r="D11" s="13" t="s">
         <v>13</v>
       </c>
@@ -2456,17 +2554,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="C4:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="4" spans="3:5">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C4" t="s">
         <v>16</v>
       </c>
@@ -2477,7 +2575,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="3:5" hidden="1">
+    <row r="5" spans="3:5" hidden="1" x14ac:dyDescent="0.15">
       <c r="C5" t="s">
         <v>17</v>
       </c>
@@ -2488,7 +2586,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="3:5">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C6" t="s">
         <v>16</v>
       </c>
@@ -2499,7 +2597,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="3:5" hidden="1">
+    <row r="7" spans="3:5" hidden="1" x14ac:dyDescent="0.15">
       <c r="C7" t="s">
         <v>18</v>
       </c>
@@ -2510,7 +2608,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="3:5" hidden="1">
+    <row r="8" spans="3:5" hidden="1" x14ac:dyDescent="0.15">
       <c r="C8" t="s">
         <v>17</v>
       </c>
@@ -2518,7 +2616,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="3:5">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C9" t="s">
         <v>19</v>
       </c>
@@ -2526,7 +2624,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="3:5">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C10" t="s">
         <v>19</v>
       </c>
@@ -2537,7 +2635,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="3:5">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C11" t="s">
         <v>20</v>
       </c>
@@ -2564,16 +2662,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="4" spans="3:5">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C4" t="s">
         <v>16</v>
       </c>
@@ -2584,7 +2682,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="3:5">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C5" t="s">
         <v>17</v>
       </c>
@@ -2595,7 +2693,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="3:5">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C6" t="s">
         <v>16</v>
       </c>
@@ -2606,7 +2704,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="3:5">
+    <row r="7" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C7" t="s">
         <v>18</v>
       </c>
@@ -2617,7 +2715,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="3:5">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C8" t="s">
         <v>17</v>
       </c>
@@ -2625,7 +2723,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="3:5">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C9" t="s">
         <v>19</v>
       </c>
@@ -2633,7 +2731,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="3:5">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C10" t="s">
         <v>19</v>
       </c>
@@ -2644,7 +2742,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="3:5">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C11" t="s">
         <v>20</v>
       </c>
@@ -2662,16 +2760,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.15">
       <c r="C2" s="19" t="s">
         <v>40</v>
       </c>
@@ -2685,7 +2783,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="2:6">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B3" s="19" t="s">
         <v>30</v>
       </c>
@@ -2703,7 +2801,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B4" s="19" t="s">
         <v>31</v>
       </c>
@@ -2721,7 +2819,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B5" s="19" t="s">
         <v>32</v>
       </c>
@@ -2739,7 +2837,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B6" s="19" t="s">
         <v>33</v>
       </c>
@@ -2757,7 +2855,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B7" s="19" t="s">
         <v>34</v>
       </c>
@@ -2775,7 +2873,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B8" s="19" t="s">
         <v>35</v>
       </c>
@@ -2793,7 +2891,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B9" s="19" t="s">
         <v>36</v>
       </c>
@@ -2811,7 +2909,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B10" s="19" t="s">
         <v>37</v>
       </c>
@@ -2829,7 +2927,7 @@
         <v>1723</v>
       </c>
     </row>
-    <row r="11" spans="2:6">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B11" s="19" t="s">
         <v>38</v>
       </c>
@@ -2847,7 +2945,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B12" s="19" t="s">
         <v>39</v>
       </c>
@@ -2872,16 +2970,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.15">
       <c r="C2" s="19" t="s">
         <v>40</v>
       </c>
@@ -2895,7 +2993,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="2:6">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B3" s="19" t="s">
         <v>30</v>
       </c>
@@ -2913,7 +3011,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B4" s="19" t="s">
         <v>31</v>
       </c>
@@ -2931,7 +3029,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B5" s="19" t="s">
         <v>32</v>
       </c>
@@ -2949,7 +3047,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B6" s="19" t="s">
         <v>33</v>
       </c>
@@ -2967,7 +3065,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B7" s="19" t="s">
         <v>34</v>
       </c>
@@ -2985,7 +3083,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B8" s="19" t="s">
         <v>35</v>
       </c>
@@ -3003,7 +3101,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B9" s="19" t="s">
         <v>36</v>
       </c>
@@ -3021,7 +3119,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B10" s="19" t="s">
         <v>37</v>
       </c>
@@ -3039,7 +3137,7 @@
         <v>1723</v>
       </c>
     </row>
-    <row r="11" spans="2:6">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B11" s="19" t="s">
         <v>38</v>
       </c>
@@ -3057,7 +3155,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B12" s="19" t="s">
         <v>39</v>
       </c>
@@ -3083,21 +3181,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="e">
         <f ca="1">XYZ()</f>
         <v>#NAME?</v>
@@ -3112,7 +3210,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -3126,9 +3224,9 @@
         <v>99.99</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -3140,7 +3238,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B5">
         <f>SUM(B1:B3)</f>
         <v>6</v>

</xml_diff>